<commit_message>
Updated multiple files and added new scripts for AI project
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\atom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4EC085-A025-45AD-8F43-8BE48FF9F050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C1B5F9-C5FC-4A7B-B810-DD4D9932A89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{28990DF4-71CB-4E69-BE07-0C6EBD0AC1C1}"/>
   </bookViews>
@@ -67,22 +67,22 @@
     <t>are you fine</t>
   </si>
   <si>
-    <t>get set</t>
-  </si>
-  <si>
-    <t>I am fine,thank you sir</t>
-  </si>
-  <si>
     <t>yes I am fine sir</t>
   </si>
   <si>
-    <t>I am ready sir</t>
-  </si>
-  <si>
     <t>are you ok</t>
   </si>
   <si>
-    <t>yes sir,I am fine</t>
+    <t>I am rgood sir</t>
+  </si>
+  <si>
+    <t>are you set</t>
+  </si>
+  <si>
+    <t>I am fine thank you sir</t>
+  </si>
+  <si>
+    <t>yes sir I am fine</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,13 +468,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,16 +514,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>